<commit_message>
1.0.1 Signed-off-by: HY-ZhengWei <HY.ZhengWei@qq.com>
</commit_message>
<xml_diff>
--- a/test/org/hy/common/report/junit/JU_Report01.xlsx
+++ b/test/org/hy/common/report/junit/JU_Report01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="80" windowWidth="25280" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,41 @@
     <author xml:space="preserve">  ZhengWei(HY)</author>
   </authors>
   <commentList>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">  ZhengWei(HY):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Hello </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="10"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>World</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A5" authorId="0">
       <text>
         <r>
@@ -46,7 +81,26 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-通过自定义事件，实现动态图片的显示</t>
+通过</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="53"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>自定义事件</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t>，实现动态图片的显示</t>
         </r>
       </text>
     </comment>
@@ -72,7 +126,16 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-此为系统变量</t>
+此为</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="49"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>系统变量</t>
         </r>
       </text>
     </comment>
@@ -102,6 +165,41 @@
         </r>
       </text>
     </comment>
+    <comment ref="F20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">  ZhengWei(HY):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+为什么要在这里放一个</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="14"/>
+            <color indexed="10"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>水果</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -155,31 +253,33 @@
     <r>
       <rPr>
         <sz val="24"/>
-        <color theme="1"/>
+        <color indexed="8"/>
         <rFont val="宋体"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t>标题</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>合计：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>:RowCount__</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:RowNo__</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
       <rPr>
         <sz val="16"/>
-        <color theme="1"/>
+        <color indexed="8"/>
         <rFont val="宋体"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t>谢谢</t>
     </r>
@@ -197,11 +297,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>:image</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>:RowNo__</t>
+    <t>合计：</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -209,7 +305,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -223,39 +319,12 @@
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="24"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -272,6 +341,36 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="49"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="53"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="10"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="10"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -281,7 +380,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -293,15 +392,120 @@
       <left style="medium">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
       <top style="medium">
         <color auto="1"/>
@@ -351,6 +555,26 @@
     </border>
     <border>
       <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top/>
       <bottom style="medium">
@@ -363,209 +587,120 @@
       <right style="medium">
         <color auto="1"/>
       </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -590,18 +725,25 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="图片 3"/>
+        <xdr:cNvPr id="1058" name="图片 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="228600" y="50800"/>
           <a:ext cx="1231900" cy="1231900"/>
@@ -609,6 +751,165 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1422400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1059" name="图片 3" descr="HY标志.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4140200" y="2921000"/>
+          <a:ext cx="1409700" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1625600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2108200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1060" name="图片 1" descr="u=3898195537,322862068&amp;fm=23&amp;gp=0.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5753100" y="4521200"/>
+          <a:ext cx="482600" cy="469900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -941,7 +1242,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -950,62 +1251,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="8"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="35" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="10"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="35" customHeight="1" thickBot="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="12"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" ht="20" customHeight="1" thickBot="1">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="7" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="8"/>
+      <c r="A5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1014,10 +1315,10 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="9"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1026,10 +1327,10 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="9"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1038,109 +1339,129 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="9"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="16" thickBot="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="9"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="9"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="9"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="9"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="9"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="9"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="9"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="9"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="10"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" ht="16" thickBot="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:6" ht="16" thickBot="1">
-      <c r="A20" s="16" t="s">
+      <c r="A19" s="19"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" ht="22" customHeight="1" thickBot="1">
+      <c r="A20" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:6" ht="20" thickBot="1">
-      <c r="A21" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="27"/>
+    </row>
+    <row r="21" spans="1:6" ht="22" customHeight="1" thickBot="1">
+      <c r="A21" s="19"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="E11:F19"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="C1:F3"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="A21:F21"/>
     <mergeCell ref="A5:D19"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="C20:E20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
1.0.2 Signed-off-by: HY-ZhengWei <HY.ZhengWei@qq.com>
</commit_message>
<xml_diff>
--- a/test/org/hy/common/report/junit/JU_Report01.xlsx
+++ b/test/org/hy/common/report/junit/JU_Report01.xlsx
@@ -664,77 +664,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
@@ -1278,7 +1278,8 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1288,204 +1289,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="8"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" ht="35" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="10"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" spans="1:6" ht="35" customHeight="1" thickBot="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="12"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="20" customHeight="1" thickBot="1">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="7" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="8"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="9"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="21"/>
       <c r="E7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="9"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="21"/>
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="9"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="31"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" ht="16" thickBot="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="9"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="9"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="9"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="24"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="9"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="9"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="9"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="24"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="9"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="24"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="9"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="1:6" ht="16" thickBot="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" ht="22" customHeight="1" thickBot="1">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="24"/>
+      <c r="C20" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="19"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="30"/>
     </row>
     <row r="21" spans="1:6" ht="22" customHeight="1" thickBot="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="5" t="s">
+      <c r="A21" s="22"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="20"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>